<commit_message>
Multi İntercom URL uzantısı eklendi.
</commit_message>
<xml_diff>
--- a/pages/haberlesme.xlsx
+++ b/pages/haberlesme.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EARGE8PC\Desktop\btk42GithubIo\pages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTK\Butkon\Projeler\BTK42_EXCEL\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF6446-DAF5-407D-BC2D-0EBDB5730769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="43">
   <si>
     <t>Sıra</t>
   </si>
@@ -150,13 +151,16 @@
   </si>
   <si>
     <t>Model-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/CM-MLI-00-000-000-P1B1-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -186,6 +190,14 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,10 +232,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -243,8 +256,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -541,7 +558,7 @@
     <col min="8" max="8" width="15.21875" style="6" customWidth="1"/>
     <col min="9" max="9" width="18.5546875" style="6" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="39.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="55.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
@@ -842,7 +859,9 @@
       <c r="J9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -911,8 +930,11 @@
       <c r="K11" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K9" r:id="rId1" xr:uid="{473CCB9F-9F6A-4388-BAD8-F0D74455EE1C}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>